<commit_message>
Add complete From field (prevents classification as spam!)
</commit_message>
<xml_diff>
--- a/py_bulk_email.xlsx
+++ b/py_bulk_email.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t xml:space="preserve">secondary email field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sender name</t>
   </si>
   <si>
     <t xml:space="preserve">html</t>
@@ -302,18 +308,18 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.5280898876404"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.9719101123596"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="72.2415730337079"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="55"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="39.8370786516854"/>
-    <col collapsed="false" hidden="false" max="1021" min="6" style="1" width="22.2977528089888"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="22.2977528089888"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.0674157303371"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="42.5112359550562"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="85.4719101123596"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="65.1067415730337"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="47.2696629213483"/>
+    <col collapsed="false" hidden="false" max="1021" min="6" style="1" width="26.3089887640449"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="26.3089887640449"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -387,17 +393,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:4"/>
+  <dimension ref="1:5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="30.1741573033708"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="166.331460674157"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.2584269662921"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="35.5280898876404"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="197.101123595506"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -427,12 +432,21 @@
       </c>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="387.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>13</v>
+      </c>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="387.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -453,49 +467,48 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="58.2696629213483"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="49.7977528089888"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="49.7977528089888"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.5786516853933"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.5393258426966"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.2584269662921"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="68.9719101123596"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="59.0112359550562"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="59.0112359550562"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.0112359550562"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.7415730337079"/>
   </cols>
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E2" s="13" t="n">
         <v>465</v>

</xml_diff>